<commit_message>
Added test cases for Login, HomePage, ExpenseCategory
</commit_message>
<xml_diff>
--- a/src/main/java/Resource/DataValues.xlsx
+++ b/src/main/java/Resource/DataValues.xlsx
@@ -7,19 +7,39 @@
     <workbookView windowWidth="22368" windowHeight="9215"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="5" r:id="rId1"/>
+    <sheet name="LoginCredentials" sheetId="5" r:id="rId1"/>
+    <sheet name="LoginSuccess" sheetId="7" r:id="rId2"/>
+    <sheet name="LogOutSucess" sheetId="8" r:id="rId3"/>
+    <sheet name="ExpenseCategoryName" sheetId="9" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>https://groceryapp.uniqassosiates.com/admin</t>
+  </si>
+  <si>
+    <t>https://groceryapp.uniqassosiates.com/admin/login</t>
+  </si>
+  <si>
+    <t>FreshJuice</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -30,8 +50,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -44,23 +72,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -68,7 +81,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -90,6 +103,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -107,14 +127,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -130,6 +142,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -139,14 +158,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -154,6 +166,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -161,14 +181,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -183,187 +203,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -374,6 +394,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -416,21 +451,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -457,6 +477,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -465,165 +494,157 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -943,14 +964,98 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="1"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="42.8888888888889" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" display="https://groceryapp.uniqassosiates.com/admin" tooltip="https://groceryapp.uniqassosiates.com/admin"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="44.7777777777778" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>

<commit_message>
twenty six test case passed
</commit_message>
<xml_diff>
--- a/src/main/java/Resource/DataValues.xlsx
+++ b/src/main/java/Resource/DataValues.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22368" windowHeight="9215" firstSheet="2" activeTab="3"/>
+    <workbookView windowWidth="22368" windowHeight="9215" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="5" r:id="rId1"/>
@@ -15,13 +15,16 @@
     <sheet name="ManageDeliveryBoy" sheetId="11" r:id="rId6"/>
     <sheet name="Settings" sheetId="12" r:id="rId7"/>
     <sheet name="PushNotification" sheetId="13" r:id="rId8"/>
+    <sheet name="ManageUser" sheetId="15" r:id="rId9"/>
+    <sheet name="AdminUsers" sheetId="16" r:id="rId10"/>
+    <sheet name="ManageSlider" sheetId="17" r:id="rId11"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
   <si>
     <t>admin</t>
   </si>
@@ -50,6 +53,24 @@
     <t>Manage Expense</t>
   </si>
   <si>
+    <t>Manage Users</t>
+  </si>
+  <si>
+    <t>Admin Users</t>
+  </si>
+  <si>
+    <t>Manage Slider</t>
+  </si>
+  <si>
+    <t>Push Notifications</t>
+  </si>
+  <si>
+    <t>Settings</t>
+  </si>
+  <si>
+    <t>Expense Category</t>
+  </si>
+  <si>
     <t>Vicky</t>
   </si>
   <si>
@@ -102,6 +123,21 @@
   </si>
   <si>
     <t>Amul</t>
+  </si>
+  <si>
+    <t>Jishnu V</t>
+  </si>
+  <si>
+    <t>Akshatha</t>
+  </si>
+  <si>
+    <t>Aks123</t>
+  </si>
+  <si>
+    <t>https://groceryapp.uniqassosiates.com/admin/list-slider</t>
+  </si>
+  <si>
+    <t>https://groceryapp.uniqassosiates.com/admin/Slider/add</t>
   </si>
 </sst>
 </file>
@@ -109,18 +145,24 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF212529"/>
+      <name val="Segoe UI"/>
+      <charset val="134"/>
     </font>
     <font>
       <u/>
@@ -137,6 +179,20 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -146,14 +202,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -167,24 +224,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -198,13 +239,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -223,6 +257,36 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -231,14 +295,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -246,21 +303,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -288,18 +330,120 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -312,61 +456,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -378,66 +498,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -445,24 +505,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -476,22 +518,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -511,6 +548,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -526,17 +572,31 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -555,182 +615,165 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1076,6 +1119,71 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2"/>
+  <cols>
+    <col min="1" max="1" width="15.5555555555556" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="19.2" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="51.8888888888889" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
@@ -1091,7 +1199,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1134,7 +1242,7 @@
   <sheetPr/>
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -1164,26 +1272,26 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="62" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="50" customHeight="1" spans="1:6">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
@@ -1191,8 +1299,48 @@
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1219,59 +1367,59 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>16</v>
+      <c r="A3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
@@ -1319,12 +1467,12 @@
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1349,17 +1497,39 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" ht="19.2" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
twenty six final commit
</commit_message>
<xml_diff>
--- a/src/main/java/Resource/DataValues.xlsx
+++ b/src/main/java/Resource/DataValues.xlsx
@@ -145,8 +145,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
@@ -180,6 +180,20 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -193,6 +207,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -201,10 +223,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -247,69 +270,46 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -324,79 +324,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -408,103 +498,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -518,17 +518,29 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -548,15 +560,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -572,11 +575,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -588,15 +597,6 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -618,148 +618,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>

</xml_diff>

<commit_message>
Testcase for Second Demo
</commit_message>
<xml_diff>
--- a/src/main/java/Resource/DataValues.xlsx
+++ b/src/main/java/Resource/DataValues.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22368" windowHeight="9215" activeTab="4"/>
+    <workbookView windowWidth="22368" windowHeight="9215" firstSheet="3" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="5" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
   <si>
     <t>admin</t>
   </si>
@@ -35,13 +35,13 @@
     <t>https://groceryapp.uniqassosiates.com/admin/login</t>
   </si>
   <si>
-    <t>FreshJuice</t>
-  </si>
-  <si>
-    <t>Dummy</t>
-  </si>
-  <si>
-    <t>Mango Mojito</t>
+    <t>everydaymilkpowder</t>
+  </si>
+  <si>
+    <t>dummyTest</t>
+  </si>
+  <si>
+    <t>nido</t>
   </si>
   <si>
     <t>https://groceryapp.uniqassosiates.com/admin/expense-category</t>
@@ -71,49 +71,70 @@
     <t>Expense Category</t>
   </si>
   <si>
-    <t>Vicky</t>
-  </si>
-  <si>
-    <t>Kiran</t>
-  </si>
-  <si>
-    <t>vicky95@gmail.com</t>
-  </si>
-  <si>
-    <t>Dummy@gmail.com</t>
-  </si>
-  <si>
-    <t>Kiran@gmail.com</t>
-  </si>
-  <si>
-    <t>7896541230</t>
-  </si>
-  <si>
-    <t>999999999</t>
-  </si>
-  <si>
-    <t>8888888888</t>
-  </si>
-  <si>
-    <t>trivandrum</t>
-  </si>
-  <si>
-    <t>Chennai</t>
-  </si>
-  <si>
-    <t>Vicky1995</t>
-  </si>
-  <si>
-    <t>Dummy123</t>
+    <t>Manage Menu</t>
+  </si>
+  <si>
+    <t>manu</t>
+  </si>
+  <si>
+    <t>testedit</t>
+  </si>
+  <si>
+    <t>Kannan</t>
+  </si>
+  <si>
+    <t>manu1895@gmail.com</t>
+  </si>
+  <si>
+    <t>edittest@gmail.com</t>
+  </si>
+  <si>
+    <t>Kiannan@gmail.com</t>
+  </si>
+  <si>
+    <t>7478523690</t>
+  </si>
+  <si>
+    <t>555555555555</t>
+  </si>
+  <si>
+    <t>741258963654</t>
+  </si>
+  <si>
+    <t>tvm</t>
+  </si>
+  <si>
+    <t>kollam</t>
+  </si>
+  <si>
+    <t>manu91</t>
+  </si>
+  <si>
+    <t>qpweiruyt</t>
+  </si>
+  <si>
+    <t>http://groceryapp.uniqassosiates.com/admin/login</t>
+  </si>
+  <si>
+    <t>TestingAutomationDemo</t>
+  </si>
+  <si>
+    <t>https://groceryapp.uniqassosiatess.com/admin/verify-users</t>
+  </si>
+  <si>
+    <t>fa-cutlery</t>
+  </si>
+  <si>
+    <t>1111</t>
+  </si>
+  <si>
+    <t>DemoTest</t>
   </si>
   <si>
     <t>qwerty</t>
   </si>
   <si>
-    <t>http://groceryapp.uniqassosiates.com/admin/login</t>
-  </si>
-  <si>
-    <t>fa-cutlery</t>
+    <t>Green</t>
   </si>
   <si>
     <t>https://groceryapp.uniqassosiates.com/admin/list-notifications</t>
@@ -128,10 +149,13 @@
     <t>Jishnu V</t>
   </si>
   <si>
-    <t>Akshatha</t>
-  </si>
-  <si>
-    <t>Aks123</t>
+    <t>rgba(255, 255, 255, 1)</t>
+  </si>
+  <si>
+    <t>Akshaya</t>
+  </si>
+  <si>
+    <t>Aky123</t>
   </si>
   <si>
     <t>https://groceryapp.uniqassosiates.com/admin/list-slider</t>
@@ -145,10 +169,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -173,6 +197,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="9"/>
       <color rgb="FF202124"/>
       <name val="Consolas"/>
@@ -180,20 +212,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -202,6 +220,67 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -215,9 +294,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -231,61 +309,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -299,15 +332,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -324,187 +348,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -518,29 +542,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -560,6 +572,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -571,6 +592,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -601,179 +631,175 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1135,17 +1161,17 @@
   <sheetData>
     <row r="1" ht="19.2" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1170,12 +1196,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1199,7 +1225,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="7" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1243,12 +1269,13 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="11.2222222222222" customWidth="1"/>
+    <col min="1" max="1" width="20.2222222222222" customWidth="1"/>
+    <col min="2" max="2" width="12.7777777777778" customWidth="1"/>
     <col min="3" max="3" width="17.6666666666667" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1272,10 +1299,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
@@ -1284,14 +1311,14 @@
   </cols>
   <sheetData>
     <row r="1" ht="50" customHeight="1" spans="1:6">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
@@ -1299,12 +1326,12 @@
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1314,7 +1341,7 @@
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="6" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1341,6 +1368,11 @@
     <row r="11" spans="1:1">
       <c r="A11" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1355,81 +1387,81 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="17.7777777777778" customWidth="1"/>
-    <col min="2" max="2" width="10.6666666666667"/>
-    <col min="3" max="3" width="11.7777777777778"/>
+    <col min="1" max="1" width="19.8888888888889" customWidth="1"/>
+    <col min="2" max="2" width="22.3333333333333" customWidth="1"/>
+    <col min="3" max="3" width="20.6666666666667" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="B2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="7" t="s">
+      <c r="A3" s="8" t="s">
         <v>22</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="vicky95@gmail.com" tooltip="mailto:vicky95@gmail.com"/>
-    <hyperlink ref="B2" r:id="rId2" display="Dummy@gmail.com"/>
-    <hyperlink ref="C2" r:id="rId3" display="Kiran@gmail.com"/>
+    <hyperlink ref="A2" r:id="rId1" display="manu1895@gmail.com" tooltip="mailto:manu1895@gmail.com"/>
+    <hyperlink ref="B2" r:id="rId2" display="edittest@gmail.com" tooltip="mailto:edittest@gmail.com"/>
+    <hyperlink ref="C2" r:id="rId3" display="Kiannan@gmail.com" tooltip="mailto:Kiannan@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -1439,15 +1471,15 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="44.3333333333333" customWidth="1"/>
+    <col min="1" max="1" width="53.3333333333333" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -1467,15 +1499,48 @@
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="9" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A6" r:id="rId1" display="https://groceryapp.uniqassosiatess.com/admin/verify-users"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
@@ -1497,17 +1562,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1519,17 +1584,25 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="17.8888888888889" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" ht="19.2" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new test cases
</commit_message>
<xml_diff>
--- a/src/main/java/Resource/DataValues.xlsx
+++ b/src/main/java/Resource/DataValues.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22368" windowHeight="9215" firstSheet="3" activeTab="8"/>
+    <workbookView windowWidth="22368" windowHeight="9215" firstSheet="8" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="5" r:id="rId1"/>
@@ -18,13 +18,16 @@
     <sheet name="ManageUser" sheetId="15" r:id="rId9"/>
     <sheet name="AdminUsers" sheetId="16" r:id="rId10"/>
     <sheet name="ManageSlider" sheetId="17" r:id="rId11"/>
+    <sheet name="ManagePaymentMethod" sheetId="18" r:id="rId12"/>
+    <sheet name="ManageLocation" sheetId="19" r:id="rId13"/>
+    <sheet name="ManageExpense" sheetId="20" r:id="rId14"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="53">
   <si>
     <t>admin</t>
   </si>
@@ -74,6 +77,12 @@
     <t>Manage Menu</t>
   </si>
   <si>
+    <t>Manage Payment Methods</t>
+  </si>
+  <si>
+    <t>Manage Location</t>
+  </si>
+  <si>
     <t>manu</t>
   </si>
   <si>
@@ -146,7 +155,7 @@
     <t>Amul</t>
   </si>
   <si>
-    <t>Jishnu V</t>
+    <t>Florance Kurian</t>
   </si>
   <si>
     <t>rgba(255, 255, 255, 1)</t>
@@ -162,6 +171,21 @@
   </si>
   <si>
     <t>https://groceryapp.uniqassosiates.com/admin/Slider/add</t>
+  </si>
+  <si>
+    <t>SBI Debit Card</t>
+  </si>
+  <si>
+    <t>Crowbar Street</t>
+  </si>
+  <si>
+    <t>OxfordUniversity</t>
+  </si>
+  <si>
+    <t>700</t>
+  </si>
+  <si>
+    <t>Bristol</t>
   </si>
 </sst>
 </file>
@@ -169,10 +193,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -234,14 +258,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -256,6 +272,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -264,20 +287,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -294,13 +303,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -310,7 +312,44 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -323,21 +362,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -348,187 +372,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -539,21 +563,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -605,6 +614,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -620,6 +638,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -630,167 +663,158 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -798,6 +822,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" quotePrefix="1">
@@ -1151,7 +1176,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2"/>
@@ -1161,17 +1186,17 @@
   <sheetData>
     <row r="1" ht="19.2" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1196,15 +1221,101 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="17.5555555555556" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2">
+        <v>50000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="3"/>
+  <cols>
+    <col min="1" max="1" width="17.5555555555556" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
@@ -1225,7 +1336,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1269,7 +1380,7 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="2"/>
@@ -1299,10 +1410,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
@@ -1373,6 +1484,16 @@
     <row r="12" spans="1:1">
       <c r="A12" s="6" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="7" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1399,62 +1520,62 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="9" t="s">
+      <c r="A3" s="9" t="s">
         <v>24</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1499,42 +1620,42 @@
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="9" t="s">
-        <v>33</v>
+      <c r="A8" s="10" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1562,17 +1683,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1586,8 +1707,8 @@
   <sheetPr/>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1"/>
@@ -1597,12 +1718,12 @@
   <sheetData>
     <row r="1" ht="19.2" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>